<commit_message>
feat: update to deepface
</commit_message>
<xml_diff>
--- a/attendance_sheets/semester_register.xlsx
+++ b/attendance_sheets/semester_register.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Generated: 05-02-2026 07:18:27</t>
+          <t>Generated: 09-02-2026 09:23:58</t>
         </is>
       </c>
     </row>
@@ -528,12 +528,12 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>04/02</t>
+          <t>08/02</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>05/02</t>
+          <t>09/02</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>Jikmet Lama</t>
+          <t>Takap Lama</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
@@ -553,9 +553,9 @@
           <t>P</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>P</t>
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -567,12 +567,12 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>Chhakit Lama</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>A</t>
+          <t>Jikmet lama</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>P</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
@@ -589,46 +589,68 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
+          <t>Chhakit Lama</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
           <t>Sangat Maharjan</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="C7" s="5" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D7" s="5" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="7" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>Legend:</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="8" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="8" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Present</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="9" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="9" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Absent</t>
         </is>

</xml_diff>